<commit_message>
cambios en el sistema de veritas
</commit_message>
<xml_diff>
--- a/Lecturas_BureauVeritas/Lecturas_BureauVeritas/formatos/FORMATO_REPARTO.xlsx
+++ b/Lecturas_BureauVeritas/Lecturas_BureauVeritas/formatos/FORMATO_REPARTO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\FORMATOS_VERITAS_CALIDDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -268,6 +268,15 @@
   </si>
   <si>
     <t>6314L24</t>
+  </si>
+  <si>
+    <t>tipo_recibo</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -309,7 +318,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -332,18 +341,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Diseño" xfId="1"/>
@@ -649,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +694,7 @@
     <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -724,8 +746,11 @@
       <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -769,8 +794,11 @@
         <v>3</v>
       </c>
       <c r="Q2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -814,8 +842,11 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -861,8 +892,11 @@
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -908,8 +942,11 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -953,8 +990,11 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1000,8 +1040,11 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1049,8 +1092,11 @@
       <c r="Q8" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1096,8 +1142,11 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1143,8 +1192,11 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1188,8 +1240,11 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1233,8 +1288,11 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1280,8 +1338,11 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1327,8 +1388,11 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1374,8 +1438,11 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1421,8 +1488,11 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1464,8 +1534,11 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1509,8 +1582,11 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1556,8 +1632,11 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1601,6 +1680,9 @@
         <v>3</v>
       </c>
       <c r="Q20" s="4"/>
+      <c r="R20" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mantenimientos y procesos en sistema de veritas
</commit_message>
<xml_diff>
--- a/Lecturas_BureauVeritas/Lecturas_BureauVeritas/formatos/FORMATO_REPARTO.xlsx
+++ b/Lecturas_BureauVeritas/Lecturas_BureauVeritas/formatos/FORMATO_REPARTO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FUENTES_LECTURAS\Lecturas_BureauVeritas\Lecturas_BureauVeritas\Lecturas_BureauVeritas\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>impresion</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
 </sst>
 </file>
@@ -357,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -366,6 +372,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Diseño" xfId="1"/>
@@ -671,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +701,7 @@
     <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,8 +756,11 @@
       <c r="R1" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -797,8 +807,9 @@
       <c r="R2" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -845,8 +856,11 @@
       <c r="R3" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -895,8 +909,11 @@
       <c r="R4" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -945,8 +962,11 @@
       <c r="R5" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -993,8 +1013,11 @@
       <c r="R6" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1043,8 +1066,11 @@
       <c r="R7" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1095,8 +1121,11 @@
       <c r="R8" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1145,8 +1174,11 @@
       <c r="R9" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1195,8 +1227,11 @@
       <c r="R10" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1243,8 +1278,11 @@
       <c r="R11" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1291,8 +1329,11 @@
       <c r="R12" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1341,8 +1382,11 @@
       <c r="R13" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1391,8 +1435,11 @@
       <c r="R14" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1441,8 +1488,11 @@
       <c r="R15" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1491,8 +1541,9 @@
       <c r="R16" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1537,8 +1588,9 @@
       <c r="R17" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1585,8 +1637,9 @@
       <c r="R18" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1635,8 +1688,9 @@
       <c r="R19" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1683,6 +1737,7 @@
       <c r="R20" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="S20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambios en grandes clientes
</commit_message>
<xml_diff>
--- a/Lecturas_BureauVeritas/Lecturas_BureauVeritas/formatos/FORMATO_REPARTO.xlsx
+++ b/Lecturas_BureauVeritas/Lecturas_BureauVeritas/formatos/FORMATO_REPARTO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FUENTES_LECTURAS\Lecturas_BureauVeritas\Lecturas_BureauVeritas\Lecturas_BureauVeritas\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -276,13 +276,19 @@
     <t>I</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>impresion</t>
   </si>
   <si>
     <t>SI</t>
+  </si>
+  <si>
+    <t>latitud</t>
+  </si>
+  <si>
+    <t>longitud</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -316,12 +322,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -363,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -373,6 +385,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Diseño" xfId="1"/>
@@ -678,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="T1" sqref="T1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +714,7 @@
     <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -753,14 +766,20 @@
       <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="9" t="s">
         <v>82</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -808,8 +827,14 @@
         <v>83</v>
       </c>
       <c r="S2" s="8"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="7">
+        <v>-11.99226322</v>
+      </c>
+      <c r="U2" s="7">
+        <v>-77.016212699999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -857,10 +882,16 @@
         <v>83</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T3" s="7">
+        <v>-11.998517140000001</v>
+      </c>
+      <c r="U3" s="7">
+        <v>-77.015098710000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -910,10 +941,16 @@
         <v>83</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T4" s="7">
+        <v>-11.99195128</v>
+      </c>
+      <c r="U4" s="7">
+        <v>-77.016578960000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -963,10 +1000,16 @@
         <v>83</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T5" s="7">
+        <v>-11.99195128</v>
+      </c>
+      <c r="U5" s="7">
+        <v>-77.016578960000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1014,10 +1057,16 @@
         <v>83</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T6" s="7">
+        <v>-11.99370599</v>
+      </c>
+      <c r="U6" s="7">
+        <v>-77.012533450000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1067,10 +1116,16 @@
         <v>83</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T7" s="7">
+        <v>-11.996716790000001</v>
+      </c>
+      <c r="U7" s="7">
+        <v>-77.015934130000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1122,10 +1177,16 @@
         <v>83</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T8" s="7">
+        <v>-11.996716790000001</v>
+      </c>
+      <c r="U8" s="7">
+        <v>-77.015934130000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1175,10 +1236,16 @@
         <v>83</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T9" s="7">
+        <v>-11.99219227</v>
+      </c>
+      <c r="U9" s="7">
+        <v>-77.0166234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1228,10 +1295,16 @@
         <v>83</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T10" s="7">
+        <v>-11.99219227</v>
+      </c>
+      <c r="U10" s="7">
+        <v>-77.0166234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1279,10 +1352,16 @@
         <v>83</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T11" s="7">
+        <v>-11.99219227</v>
+      </c>
+      <c r="U11" s="7">
+        <v>-77.0166234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1330,10 +1409,16 @@
         <v>83</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T12" s="7">
+        <v>-11.99219227</v>
+      </c>
+      <c r="U12" s="7">
+        <v>-77.0166234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1383,10 +1468,16 @@
         <v>83</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T13" s="7">
+        <v>-11.996657969999999</v>
+      </c>
+      <c r="U13" s="7">
+        <v>-77.015911099999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1433,13 +1524,19 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T14" s="7">
+        <v>-11.996657969999999</v>
+      </c>
+      <c r="U14" s="7">
+        <v>-77.015911099999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1486,13 +1583,19 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="T15" s="7">
+        <v>-11.99194726</v>
+      </c>
+      <c r="U15" s="7">
+        <v>-77.016515279999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1539,11 +1642,17 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S16" s="8"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="7">
+        <v>-11.99194726</v>
+      </c>
+      <c r="U16" s="7">
+        <v>-77.016515279999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1586,11 +1695,17 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S17" s="8"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="7">
+        <v>-11.99194726</v>
+      </c>
+      <c r="U17" s="7">
+        <v>-77.016515279999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1635,11 +1750,17 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S18" s="8"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="7">
+        <v>-11.991934860000001</v>
+      </c>
+      <c r="U18" s="7">
+        <v>-77.016324979999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1686,11 +1807,17 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S19" s="8"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="7">
+        <v>-11.99677621</v>
+      </c>
+      <c r="U19" s="7">
+        <v>-77.015957510000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1735,9 +1862,15 @@
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S20" s="8"/>
+      <c r="T20" s="7">
+        <v>-11.99677621</v>
+      </c>
+      <c r="U20" s="7">
+        <v>-77.015957510000007</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>